<commit_message>
Update Team Project Tracking Sheets.xlsx
Updated tracking sheet
</commit_message>
<xml_diff>
--- a/Team Project Tracking Sheets.xlsx
+++ b/Team Project Tracking Sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wi5483pi/Dropbox/WSU/Software Engineering/CardGame/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ss9361mn\Documents\GitHub\CardGameVer3\CardGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8686269E-FEF0-6C4D-A9BE-A2FBBB2A351A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA1D190-2867-4E5A-A971-249A35455C3B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="11680" windowHeight="14120" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="11685" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
   <si>
     <t>Copyright - Sudharsan Iyengar - August 2017.</t>
   </si>
@@ -163,9 +163,6 @@
     <t>TestGui</t>
   </si>
   <si>
-    <t>UI</t>
-  </si>
-  <si>
     <t>Contains all information regarding a player: their score, their hand, and the sum</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>Stores the state of the game and the total score.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Uzma, Will</t>
   </si>
   <si>
@@ -215,13 +209,97 @@
   </si>
   <si>
     <t>Decomposition of components of the game and how they work together</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>Has data used to transfer between Client to Server</t>
+  </si>
+  <si>
+    <t>Contains methos used to run the server</t>
+  </si>
+  <si>
+    <t>Starts the program</t>
+  </si>
+  <si>
+    <t>Orginally meant for testing, but is now the GUI used to connect players to the game</t>
+  </si>
+  <si>
+    <t>GameGUI</t>
+  </si>
+  <si>
+    <t>Ethan, Will</t>
+  </si>
+  <si>
+    <t>GUI for the card game</t>
+  </si>
+  <si>
+    <t>How the game will work</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Discussed what each of us should do and how</t>
+  </si>
+  <si>
+    <t>Game rules</t>
+  </si>
+  <si>
+    <t>We looked over the rules for the game.</t>
+  </si>
+  <si>
+    <t>Discussed Progress</t>
+  </si>
+  <si>
+    <t>Discussed progress and what we need to finish</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>Describing my classes</t>
+  </si>
+  <si>
+    <t>GUI Model</t>
+  </si>
+  <si>
+    <t>Designed GUI model and how it should work</t>
+  </si>
+  <si>
+    <t>9/15/18- 10/2/18</t>
+  </si>
+  <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Worked on implementing the distrbuted game</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>10/6/18 - 10/7/18</t>
+  </si>
+  <si>
+    <t>Made the game work with the GUI</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>Made the game more error proof</t>
+  </si>
+  <si>
+    <t>I tested my networking stuff many times when writing the code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -782,7 +860,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -818,16 +896,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1153,46 +1234,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B5" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
     <col min="11" max="11" width="3" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13">
-      <c r="D1" s="15" t="s">
+    <row r="1" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="3" spans="2:13">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="2:13" ht="32">
+    <row r="4" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I4" t="s">
         <v>25</v>
@@ -1201,15 +1282,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" ht="48">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
         <v>2</v>
       </c>
@@ -1239,7 +1320,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:13">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -1250,7 +1331,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="2:13" ht="32">
+    <row r="8" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1342,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" s="18">
+      <c r="G8" s="16">
         <v>1</v>
       </c>
       <c r="I8" s="11"/>
@@ -1269,7 +1350,7 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -1280,7 +1361,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="2:13" ht="48">
+    <row r="10" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
@@ -1293,7 +1374,7 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
@@ -1304,20 +1385,20 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="2:13" ht="32">
+    <row r="12" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" s="8">
         <v>400</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="18">
+        <v>59</v>
+      </c>
+      <c r="G12" s="16">
         <v>0.75</v>
       </c>
       <c r="I12" s="11"/>
@@ -1325,7 +1406,7 @@
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1336,12 +1417,12 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="2:13" ht="32">
+    <row r="14" spans="2:13" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E14" s="8">
         <v>600</v>
@@ -1353,7 +1434,7 @@
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1364,7 +1445,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="2:13" ht="48">
+    <row r="16" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C16" s="7" t="s">
         <v>11</v>
       </c>
@@ -1385,23 +1466,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="32">
+    <row r="3" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="12" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="32">
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>30</v>
       </c>
@@ -1412,7 +1493,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="32">
+    <row r="7" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>36</v>
       </c>
@@ -1420,126 +1501,144 @@
         <v>41</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="32">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="16">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="2:4" ht="16">
+        <v>62</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-    </row>
-    <row r="13" spans="2:4" ht="16">
+      <c r="C12" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="2:4" ht="16">
+      <c r="C13" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="2:4" ht="16">
+      <c r="C14" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="2:4" ht="80">
+        <v>66</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -1554,29 +1653,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C2:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="5" width="14.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="9.1640625" style="1"/>
+    <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7">
-      <c r="C2" s="16" t="s">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="4" spans="3:7" ht="32">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="4" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
@@ -1593,15 +1692,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="80">
-      <c r="C5" s="17">
+    <row r="5" spans="3:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="C5" s="15">
         <v>43357</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" s="8">
         <v>120</v>
@@ -1610,140 +1709,177 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="3:7">
+    <row r="6" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C6" s="19">
+        <v>43346</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="8">
+        <v>80</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C7" s="19">
+        <v>43363</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="8">
+        <v>30</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C8" s="19">
+        <v>43376</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="8">
+        <v>240</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="3:7">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="3:7">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1763,33 +1899,33 @@
   <dimension ref="C2:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="3" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7">
-      <c r="C2" s="16" t="s">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="3:7">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="3:7" ht="32">
+    <row r="4" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
@@ -1806,154 +1942,174 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="3:7">
+    <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C5" s="19">
+        <v>43356</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="8">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C6" s="19">
+        <v>43359</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="8">
+        <v>60</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="3:7">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="3:7">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="3:7">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1972,34 +2128,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C3:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="3" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="16" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="32">
+    <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
@@ -2016,164 +2172,194 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="112">
+    <row r="6" spans="3:7" ht="105" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F6" s="8">
         <v>1080</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="3:7">
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="3:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1770</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="8">
+        <v>380</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="15">
+        <v>43387</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="8">
+        <v>300</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="3:7">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="3:7">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -2193,35 +2379,35 @@
   <dimension ref="C3:G27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="16" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="32">
+    <row r="5" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
@@ -2238,154 +2424,160 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="3:7">
+      <c r="G6" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="3:7">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="3:7">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="3:7">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="3:7">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
@@ -2408,30 +2600,30 @@
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="16" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" ht="32">
+    <row r="5" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
@@ -2448,154 +2640,154 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:7">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="3:7">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="7"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="3:7">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="3:7">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="3:7">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="3:7">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="3:7">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="3:7">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="3:7">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="3:7">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="3:7">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="3:7">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="3:7">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="3:7">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="3:7">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="7"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="3:7">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="3:7">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="3:7">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="3:7">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="3:7">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="3:7">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>

</xml_diff>

<commit_message>
Sheet Changes and Manual
</commit_message>
<xml_diff>
--- a/Team Project Tracking Sheets.xlsx
+++ b/Team Project Tracking Sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ss9361mn\Documents\GitHub\CardGameVer3\CardGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wg2006qy\Documents\GitHub\CardGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1E7B15-B4CE-4B56-B8DF-79C532F17CBA}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3076A3-1CBF-4D55-B3E8-C6C0A7F0378E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="11685" windowHeight="14115" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="11685" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="109">
   <si>
     <t>Copyright - Sudharsan Iyengar - August 2017.</t>
   </si>
@@ -193,9 +193,6 @@
     <t>15 hours</t>
   </si>
   <si>
-    <t>10 hours</t>
-  </si>
-  <si>
     <t>GamePlay logic</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
     <t>Has data used to transfer between Client to Server</t>
   </si>
   <si>
-    <t>Contains methos used to run the server</t>
-  </si>
-  <si>
     <t>Starts the program</t>
   </si>
   <si>
@@ -326,6 +320,39 @@
   </si>
   <si>
     <t>Gunner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Made Small Changes to GUI </t>
+  </si>
+  <si>
+    <t>Added a auto scroll feature for testing purposes</t>
+  </si>
+  <si>
+    <t>Card Game Manual</t>
+  </si>
+  <si>
+    <t>Created Manual to allow easy use of the game</t>
+  </si>
+  <si>
+    <t>Will, Gunner</t>
+  </si>
+  <si>
+    <t>Contains methods used to run the server</t>
+  </si>
+  <si>
+    <t>#####</t>
+  </si>
+  <si>
+    <t>Double checked and tested all features of the game and made sure all requirements were met</t>
+  </si>
+  <si>
+    <t>Tested game making sure it met all requirements</t>
+  </si>
+  <si>
+    <t>10 Hours</t>
+  </si>
+  <si>
+    <t>12 hours</t>
   </si>
 </sst>
 </file>
@@ -1267,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J8" s="11"/>
       <c r="L8" s="11"/>
@@ -1433,15 +1460,17 @@
         <v>400</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" s="16">
         <v>0.75</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="J12" s="11"/>
+        <v>97</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
     </row>
@@ -1461,7 +1490,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="E14" s="8">
         <v>600</v>
@@ -1469,7 +1498,7 @@
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="I14" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J14" s="11"/>
       <c r="L14" s="11"/>
@@ -1507,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,10 +1612,10 @@
         <v>40</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
@@ -1594,10 +1623,10 @@
         <v>42</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -1605,10 +1634,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
@@ -1616,21 +1645,21 @@
         <v>44</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>68</v>
-      </c>
       <c r="D15" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="90" x14ac:dyDescent="0.25">
@@ -1644,10 +1673,16 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
+    <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
@@ -1694,7 +1729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C2:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1738,7 +1773,7 @@
         <v>43357</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>46</v>
@@ -1755,16 +1790,16 @@
         <v>43346</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F6" s="8">
         <v>80</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="60" x14ac:dyDescent="0.25">
@@ -1772,16 +1807,16 @@
         <v>43363</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F7" s="8">
         <v>30</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="60" x14ac:dyDescent="0.25">
@@ -1789,16 +1824,16 @@
         <v>43376</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F8" s="8">
         <v>240</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
@@ -1939,7 +1974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C2:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1988,16 +2023,16 @@
         <v>43356</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="8">
         <v>20</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="45" x14ac:dyDescent="0.25">
@@ -2005,16 +2040,16 @@
         <v>43359</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="8">
         <v>60</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
@@ -2169,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C3:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,10 +2250,10 @@
     </row>
     <row r="6" spans="3:7" ht="105" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>46</v>
@@ -2227,41 +2262,41 @@
         <v>1080</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="8">
         <v>1770</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="8">
         <v>380</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
@@ -2269,33 +2304,33 @@
         <v>43387</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="8">
         <v>300</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="3:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="F10" s="8">
         <v>1000</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="3:7" ht="60" x14ac:dyDescent="0.25">
@@ -2303,24 +2338,34 @@
         <v>43377</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F11" s="8">
         <v>120</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C12" s="15">
+        <v>43377</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="8">
+        <v>15</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
@@ -2439,14 +2484,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C3:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
@@ -2488,14 +2533,14 @@
     <row r="6" spans="3:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="60" x14ac:dyDescent="0.25">
@@ -2503,24 +2548,34 @@
         <v>43388</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="8">
         <v>60</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="C8" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="8">
+        <v>60</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
@@ -2667,7 +2722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E7" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
@@ -2716,16 +2771,16 @@
         <v>43388</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="8">
         <v>60</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated tracking sheet and manual
</commit_message>
<xml_diff>
--- a/Team Project Tracking Sheets.xlsx
+++ b/Team Project Tracking Sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wg2006qy\Documents\GitHub\CardGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ss9361mn\Documents\GitHub\CardGameVer3\CardGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3076A3-1CBF-4D55-B3E8-C6C0A7F0378E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F7918B-228B-4C08-9CF0-D448C98EFA8B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="11685" windowHeight="14115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="11685" windowHeight="14115" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="113">
   <si>
     <t>Copyright - Sudharsan Iyengar - August 2017.</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Card Game</t>
   </si>
   <si>
-    <t>15 hours</t>
-  </si>
-  <si>
     <t>GamePlay logic</t>
   </si>
   <si>
@@ -353,6 +350,21 @@
   </si>
   <si>
     <t>12 hours</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>77 hours</t>
+  </si>
+  <si>
+    <t>33 hours</t>
+  </si>
+  <si>
+    <t>20 hours</t>
+  </si>
+  <si>
+    <t>16 hours</t>
   </si>
 </sst>
 </file>
@@ -1294,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,9 +1418,11 @@
         <v>1</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="J8" s="11"/>
+        <v>95</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
@@ -1427,14 +1441,22 @@
       <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2</v>
+      </c>
       <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
       <c r="I10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="11"/>
+      <c r="J10" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
     </row>
@@ -1454,22 +1476,22 @@
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="E12" s="8">
         <v>400</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G12" s="16">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
@@ -1490,17 +1512,21 @@
         <v>10</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E14" s="8">
         <v>600</v>
       </c>
       <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="G14" s="16">
+        <v>1</v>
+      </c>
       <c r="I14" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="J14" s="11"/>
+        <v>88</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>112</v>
+      </c>
       <c r="L14" s="11"/>
       <c r="M14" s="11"/>
     </row>
@@ -1536,7 +1562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1612,10 +1638,10 @@
         <v>40</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
@@ -1623,10 +1649,10 @@
         <v>42</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -1634,10 +1660,10 @@
         <v>43</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
@@ -1645,21 +1671,21 @@
         <v>44</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>64</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="90" x14ac:dyDescent="0.25">
@@ -1675,13 +1701,13 @@
     </row>
     <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>101</v>
-      </c>
       <c r="D17" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -1773,7 +1799,7 @@
         <v>43357</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>46</v>
@@ -1790,16 +1816,16 @@
         <v>43346</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" s="8">
         <v>80</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="60" x14ac:dyDescent="0.25">
@@ -1807,16 +1833,16 @@
         <v>43363</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="F7" s="8">
         <v>30</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="60" x14ac:dyDescent="0.25">
@@ -1824,16 +1850,16 @@
         <v>43376</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F8" s="8">
         <v>240</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
@@ -2023,16 +2049,16 @@
         <v>43356</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="8">
         <v>20</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="45" x14ac:dyDescent="0.25">
@@ -2040,16 +2066,16 @@
         <v>43359</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="8">
         <v>60</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
@@ -2250,10 +2276,10 @@
     </row>
     <row r="6" spans="3:7" ht="105" x14ac:dyDescent="0.25">
       <c r="C6" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>46</v>
@@ -2262,41 +2288,41 @@
         <v>1080</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="E7" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="8">
         <v>1770</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="8">
         <v>380</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
@@ -2304,33 +2330,33 @@
         <v>43387</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" s="8">
         <v>300</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="3:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C10" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>89</v>
       </c>
       <c r="F10" s="8">
         <v>1000</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="3:7" ht="60" x14ac:dyDescent="0.25">
@@ -2338,16 +2364,16 @@
         <v>43377</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="8">
         <v>120</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="3:7" ht="45" x14ac:dyDescent="0.25">
@@ -2355,16 +2381,16 @@
         <v>43377</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F12" s="8">
         <v>15</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
@@ -2533,14 +2559,14 @@
     <row r="6" spans="3:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="60" x14ac:dyDescent="0.25">
@@ -2548,33 +2574,33 @@
         <v>43388</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="8">
         <v>60</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C8" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F8" s="8">
         <v>60</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
@@ -2722,7 +2748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E7" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
@@ -2771,16 +2797,16 @@
         <v>43388</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="8">
         <v>60</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>